<commit_message>
feature add account balance details
</commit_message>
<xml_diff>
--- a/src/test/resources/building_balance/building_test_file.xlsx
+++ b/src/test/resources/building_balance/building_test_file.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>NÚMERO APARTAMENTO</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>JURIDICO</t>
+  </si>
+  <si>
+    <t>SALDO ANTERIOR</t>
   </si>
   <si>
     <t>OTROS</t>
@@ -382,7 +385,8 @@
     <col customWidth="1" min="7" max="7" width="17.0"/>
     <col customWidth="1" min="8" max="8" width="15.13"/>
     <col customWidth="1" min="9" max="9" width="19.88"/>
-    <col customWidth="1" min="15" max="15" width="14.0"/>
+    <col customWidth="1" min="11" max="11" width="18.63"/>
+    <col customWidth="1" min="16" max="16" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -431,10 +435,13 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6">
         <v>45301.0</v>
@@ -467,21 +474,24 @@
         <v>0.0</v>
       </c>
       <c r="L2" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="7">
         <v>237000.0</v>
       </c>
-      <c r="M2" s="7">
-        <v>0.0</v>
-      </c>
       <c r="N2" s="7">
-        <v>100000.0</v>
+        <v>0.0</v>
       </c>
       <c r="O2" s="7">
+        <v>100000.0</v>
+      </c>
+      <c r="P2" s="7">
         <v>137000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6">
         <v>45301.0</v>
@@ -514,21 +524,24 @@
         <v>0.0</v>
       </c>
       <c r="L3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="7">
         <v>237000.0</v>
       </c>
-      <c r="M3" s="7">
-        <v>0.0</v>
-      </c>
       <c r="N3" s="7">
-        <v>100000.0</v>
+        <v>0.0</v>
       </c>
       <c r="O3" s="7">
+        <v>100000.0</v>
+      </c>
+      <c r="P3" s="7">
         <v>137000.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6">
         <v>45301.0</v>
@@ -561,21 +574,24 @@
         <v>0.0</v>
       </c>
       <c r="L4" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="7">
         <v>237000.0</v>
       </c>
-      <c r="M4" s="7">
-        <v>0.0</v>
-      </c>
       <c r="N4" s="7">
-        <v>100000.0</v>
+        <v>0.0</v>
       </c>
       <c r="O4" s="7">
+        <v>100000.0</v>
+      </c>
+      <c r="P4" s="7">
         <v>137000.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6">
         <v>45301.0</v>
@@ -608,21 +624,24 @@
         <v>0.0</v>
       </c>
       <c r="L5" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="7">
         <v>237000.0</v>
       </c>
-      <c r="M5" s="7">
-        <v>0.0</v>
-      </c>
       <c r="N5" s="7">
-        <v>100000.0</v>
+        <v>0.0</v>
       </c>
       <c r="O5" s="7">
+        <v>100000.0</v>
+      </c>
+      <c r="P5" s="7">
         <v>137000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6">
         <v>45301.0</v>
@@ -655,15 +674,18 @@
         <v>0.0</v>
       </c>
       <c r="L6" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="7">
         <v>237000.0</v>
       </c>
-      <c r="M6" s="7">
-        <v>0.0</v>
-      </c>
       <c r="N6" s="7">
-        <v>100000.0</v>
+        <v>0.0</v>
       </c>
       <c r="O6" s="7">
+        <v>100000.0</v>
+      </c>
+      <c r="P6" s="7">
         <v>137000.0</v>
       </c>
     </row>

</xml_diff>